<commit_message>
Updated top actions bar and bottom menu
</commit_message>
<xml_diff>
--- a/Model/EdlightenDataModel191120.xlsx
+++ b/Model/EdlightenDataModel191120.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashrafkabir/Desktop/projects/planb/Model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CC6B8B4-773B-354C-B650-EA29C105EC83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B88FCC04-DB96-7E43-9FAC-A8741E499441}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14060" xr2:uid="{6A4AB1DA-4CE7-9445-87D3-576E46E6202C}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="184">
   <si>
     <t>Timeline_Post</t>
   </si>
@@ -55,9 +55,6 @@
     <t>Post_Time</t>
   </si>
   <si>
-    <t>Post_Author</t>
-  </si>
-  <si>
     <t>Post_Title</t>
   </si>
   <si>
@@ -539,6 +536,57 @@
   </si>
   <si>
     <t>All, SuperAdmin, Teacher, Parent, Student</t>
+  </si>
+  <si>
+    <t>Action_Title</t>
+  </si>
+  <si>
+    <t>Action_Audience</t>
+  </si>
+  <si>
+    <t>Monthly, Weekly, Daily, etc</t>
+  </si>
+  <si>
+    <t>All, Teachers, Parents etc</t>
+  </si>
+  <si>
+    <t>Submit Planner, Fees Reminder, Special Class Enrollment etc.</t>
+  </si>
+  <si>
+    <t>Action_Recurring</t>
+  </si>
+  <si>
+    <t>Action_Active</t>
+  </si>
+  <si>
+    <t>On, Off</t>
+  </si>
+  <si>
+    <t>Action_From</t>
+  </si>
+  <si>
+    <t>Action_To</t>
+  </si>
+  <si>
+    <t>Post_Pic</t>
+  </si>
+  <si>
+    <t>UserId</t>
+  </si>
+  <si>
+    <t>Post_User_Id</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>user created, user deleted, user modified, school admin deleted, school admin modified</t>
+  </si>
+  <si>
+    <t>Last_Action_Timestamp</t>
+  </si>
+  <si>
+    <t>Last_Action_Time</t>
   </si>
 </sst>
 </file>
@@ -890,10 +938,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8FB7F83-248B-7245-AE23-026846D236AF}">
-  <dimension ref="A1:E201"/>
+  <dimension ref="A1:E213"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B17"/>
+    <sheetView tabSelected="1" topLeftCell="A116" workbookViewId="0">
+      <selection activeCell="C138" sqref="C138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -905,16 +953,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" t="s">
-        <v>9</v>
-      </c>
       <c r="D1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -927,7 +975,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -935,29 +983,29 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
         <v>166</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -965,10 +1013,10 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -976,263 +1024,263 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>6</v>
+        <v>177</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>13</v>
+        <v>179</v>
       </c>
       <c r="C11" t="s">
-        <v>14</v>
+        <v>178</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>97</v>
+        <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>98</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>161</v>
+        <v>96</v>
       </c>
       <c r="C13" t="s">
-        <v>162</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>147</v>
+        <v>160</v>
       </c>
       <c r="C14" t="s">
-        <v>146</v>
+        <v>161</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>33</v>
+        <v>146</v>
       </c>
       <c r="C15" t="s">
-        <v>35</v>
+        <v>145</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>66</v>
+        <v>32</v>
       </c>
       <c r="C16" t="s">
-        <v>65</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>143</v>
+      </c>
+      <c r="C18" t="s">
         <v>144</v>
       </c>
-      <c r="C17" t="s">
-        <v>145</v>
-      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>47</v>
+      <c r="B19" t="s">
+        <v>180</v>
+      </c>
+      <c r="C19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>1</v>
+        <v>182</v>
       </c>
       <c r="C20" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B21" t="s">
-        <v>48</v>
-      </c>
-      <c r="C21" t="s">
         <v>11</v>
       </c>
-      <c r="E21" t="s">
-        <v>96</v>
-      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B22" t="s">
-        <v>49</v>
-      </c>
-      <c r="C22" t="s">
-        <v>11</v>
+      <c r="A22" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>17</v>
-      </c>
-      <c r="C24" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B28" t="s">
-        <v>3</v>
-      </c>
-      <c r="C28" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B29" t="s">
-        <v>19</v>
-      </c>
-      <c r="C29" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B30" t="s">
-        <v>20</v>
-      </c>
-      <c r="C30" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="C31" t="s">
-        <v>2</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>18</v>
+      </c>
+      <c r="C32" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>16</v>
+      <c r="B33" t="s">
+        <v>19</v>
+      </c>
+      <c r="C33" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C34" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B35" t="s">
-        <v>45</v>
-      </c>
-      <c r="C35" t="s">
-        <v>46</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B36" t="s">
-        <v>43</v>
-      </c>
-      <c r="C36" t="s">
-        <v>11</v>
-      </c>
-      <c r="D36" t="s">
-        <v>159</v>
+      <c r="A36" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C37" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="C38" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="C39" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="D39" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C40" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C41" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C42" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C43" t="s">
-        <v>11</v>
-      </c>
-      <c r="D43" t="s">
-        <v>160</v>
+        <v>10</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="C44" t="s">
         <v>10</v>
@@ -1240,7 +1288,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C45" t="s">
         <v>10</v>
@@ -1248,82 +1296,85 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C46" t="s">
-        <v>115</v>
+        <v>10</v>
+      </c>
+      <c r="D46" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B47" t="s">
+        <v>43</v>
+      </c>
+      <c r="C47" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B48" t="s">
+        <v>28</v>
+      </c>
+      <c r="C48" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B50" t="s">
-        <v>32</v>
-      </c>
-      <c r="C50" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B51" t="s">
-        <v>50</v>
-      </c>
-      <c r="C51" t="s">
-        <v>10</v>
+      <c r="B49" t="s">
+        <v>29</v>
+      </c>
+      <c r="C49" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B52" t="s">
-        <v>51</v>
-      </c>
-      <c r="C52" t="s">
-        <v>11</v>
-      </c>
-      <c r="E52" t="s">
-        <v>52</v>
+      <c r="A52" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C53" t="s">
-        <v>11</v>
-      </c>
-      <c r="E53" t="s">
-        <v>53</v>
+        <v>9</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="C54" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="C55" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="E55" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C56" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="E56" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C57" t="s">
         <v>11</v>
@@ -1331,73 +1382,84 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B58" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="C58" t="s">
-        <v>55</v>
+        <v>11</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="C59" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B60" t="s">
+        <v>37</v>
+      </c>
+      <c r="C60" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>40</v>
+      <c r="B61" t="s">
+        <v>53</v>
+      </c>
+      <c r="C61" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B62" t="s">
+        <v>3</v>
+      </c>
+      <c r="C62" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
         <v>39</v>
       </c>
-      <c r="C62" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B63" t="s">
-        <v>56</v>
-      </c>
-      <c r="C63" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B64" t="s">
-        <v>57</v>
-      </c>
-      <c r="C64" t="s">
-        <v>62</v>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B65" t="s">
+        <v>38</v>
+      </c>
+      <c r="C65" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>61</v>
+      <c r="B66" t="s">
+        <v>55</v>
+      </c>
+      <c r="C66" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B67" t="s">
+        <v>56</v>
+      </c>
+      <c r="C67" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
         <v>60</v>
       </c>
-      <c r="C67" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B68" t="s">
-        <v>64</v>
-      </c>
-      <c r="C68" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
-        <v>58</v>
+      <c r="B70" t="s">
+        <v>59</v>
+      </c>
+      <c r="C70" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
@@ -1408,142 +1470,131 @@
         <v>10</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B72" t="s">
-        <v>59</v>
-      </c>
-      <c r="C72" t="s">
-        <v>11</v>
-      </c>
-    </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B73" t="s">
-        <v>17</v>
-      </c>
-      <c r="C73" t="s">
-        <v>10</v>
+      <c r="A73" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B74" t="s">
+        <v>62</v>
+      </c>
+      <c r="C74" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
-        <v>65</v>
+      <c r="B75" t="s">
+        <v>58</v>
+      </c>
+      <c r="C75" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B76" t="s">
-        <v>66</v>
+        <v>16</v>
       </c>
       <c r="C76" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B77" t="s">
-        <v>67</v>
-      </c>
-      <c r="C77" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B78" t="s">
-        <v>68</v>
-      </c>
-      <c r="C78" t="s">
-        <v>11</v>
+      <c r="A78" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B79" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C79" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B80" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C80" t="s">
-        <v>46</v>
+        <v>10</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B81" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C81" t="s">
-        <v>11</v>
-      </c>
-      <c r="E81" t="s">
-        <v>113</v>
+        <v>10</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B82" t="s">
-        <v>3</v>
+        <v>69</v>
       </c>
       <c r="C82" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B83" t="s">
-        <v>17</v>
+        <v>70</v>
       </c>
       <c r="C83" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B84" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C84" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="E84" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B85" t="s">
+        <v>3</v>
+      </c>
+      <c r="C85" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B86" t="s">
+        <v>16</v>
+      </c>
+      <c r="C86" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A87" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B88" t="s">
-        <v>33</v>
-      </c>
-      <c r="C88" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B89" t="s">
-        <v>73</v>
-      </c>
-      <c r="C89" t="s">
-        <v>11</v>
+      <c r="B87" t="s">
+        <v>71</v>
+      </c>
+      <c r="C87" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B90" t="s">
-        <v>79</v>
-      </c>
-      <c r="C90" t="s">
-        <v>11</v>
+      <c r="A90" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B91" t="s">
-        <v>89</v>
+        <v>32</v>
       </c>
       <c r="C91" t="s">
-        <v>90</v>
+        <v>9</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B92" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C92" t="s">
         <v>10</v>
@@ -1551,150 +1602,150 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B93" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C93" t="s">
-        <v>46</v>
+        <v>10</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B94" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="C94" t="s">
-        <v>46</v>
+        <v>89</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B95" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="C95" t="s">
-        <v>85</v>
+        <v>9</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B96" t="s">
-        <v>17</v>
+        <v>74</v>
       </c>
       <c r="C96" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B97" t="s">
-        <v>3</v>
+        <v>75</v>
       </c>
       <c r="C97" t="s">
-        <v>10</v>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B98" t="s">
+        <v>82</v>
+      </c>
+      <c r="C98" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A99" t="s">
-        <v>77</v>
+      <c r="B99" t="s">
+        <v>16</v>
+      </c>
+      <c r="C99" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B100" t="s">
-        <v>74</v>
+        <v>3</v>
       </c>
       <c r="C100" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B101" t="s">
-        <v>78</v>
-      </c>
-      <c r="C101" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B102" t="s">
-        <v>3</v>
-      </c>
-      <c r="C102" t="s">
-        <v>10</v>
+      <c r="A102" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B103" t="s">
+        <v>73</v>
+      </c>
+      <c r="C103" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A104" t="s">
-        <v>80</v>
+      <c r="B104" t="s">
+        <v>77</v>
+      </c>
+      <c r="C104" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B105" t="s">
-        <v>78</v>
+        <v>3</v>
       </c>
       <c r="C105" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B106" t="s">
-        <v>81</v>
-      </c>
-      <c r="C106" t="s">
-        <v>82</v>
+        <v>9</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B107" t="s">
-        <v>17</v>
-      </c>
-      <c r="C107" t="s">
-        <v>10</v>
+      <c r="A107" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B108" t="s">
-        <v>3</v>
+        <v>77</v>
       </c>
       <c r="C108" t="s">
-        <v>10</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B109" t="s">
+        <v>80</v>
+      </c>
+      <c r="C109" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A110" t="s">
-        <v>84</v>
+      <c r="B110" t="s">
+        <v>16</v>
+      </c>
+      <c r="C110" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B111" t="s">
-        <v>86</v>
+        <v>3</v>
       </c>
       <c r="C111" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B112" t="s">
-        <v>87</v>
-      </c>
-      <c r="C112" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B113" t="s">
-        <v>88</v>
-      </c>
-      <c r="C113" t="s">
-        <v>46</v>
+      <c r="A113" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B114" t="s">
-        <v>143</v>
+        <v>85</v>
       </c>
       <c r="C114" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B115" t="s">
-        <v>17</v>
+        <v>86</v>
       </c>
       <c r="C115" t="s">
         <v>10</v>
@@ -1702,107 +1753,118 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B116" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C116" t="s">
-        <v>90</v>
+        <v>45</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B117" t="s">
-        <v>92</v>
+        <v>142</v>
       </c>
       <c r="C117" t="s">
-        <v>11</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B118" t="s">
+        <v>16</v>
+      </c>
+      <c r="C118" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B119" t="s">
+        <v>90</v>
+      </c>
+      <c r="C119" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A120" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B121" t="s">
-        <v>2</v>
-      </c>
-      <c r="C121" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B122" t="s">
-        <v>93</v>
-      </c>
-      <c r="C122" t="s">
-        <v>11</v>
+      <c r="B120" t="s">
+        <v>91</v>
+      </c>
+      <c r="C120" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B123" t="s">
-        <v>94</v>
-      </c>
-      <c r="C123" t="s">
-        <v>11</v>
+      <c r="A123" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B124" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A128" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B129" t="s">
-        <v>100</v>
-      </c>
-      <c r="C129" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B130" t="s">
-        <v>101</v>
-      </c>
-      <c r="C130" t="s">
-        <v>46</v>
+        <v>2</v>
+      </c>
+      <c r="C124" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B125" t="s">
+        <v>92</v>
+      </c>
+      <c r="C125" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B126" t="s">
+        <v>93</v>
+      </c>
+      <c r="C126" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B127" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B131" t="s">
-        <v>102</v>
-      </c>
-      <c r="C131" t="s">
-        <v>11</v>
+      <c r="A131" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B132" t="s">
-        <v>17</v>
+        <v>99</v>
       </c>
       <c r="C132" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B133" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C133" t="s">
-        <v>98</v>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B134" t="s">
+        <v>101</v>
+      </c>
+      <c r="C134" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A135" t="s">
-        <v>103</v>
+      <c r="B135" t="s">
+        <v>16</v>
+      </c>
+      <c r="C135" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B136" t="s">
-        <v>105</v>
+        <v>180</v>
       </c>
       <c r="C136" t="s">
         <v>10</v>
@@ -1810,7 +1872,7 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B137" t="s">
-        <v>106</v>
+        <v>183</v>
       </c>
       <c r="C137" t="s">
         <v>11</v>
@@ -1818,220 +1880,220 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B138" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C138" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B139" t="s">
-        <v>109</v>
-      </c>
-      <c r="C139" t="s">
-        <v>10</v>
+        <v>97</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B140" t="s">
-        <v>110</v>
-      </c>
-      <c r="C140" t="s">
-        <v>46</v>
+      <c r="A140" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B141" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="C141" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B142" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C142" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B143" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="C143" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A146" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B144" t="s">
+        <v>108</v>
+      </c>
+      <c r="C144" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B145" t="s">
+        <v>109</v>
+      </c>
+      <c r="C145" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B146" t="s">
+        <v>111</v>
+      </c>
+      <c r="C146" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B147" t="s">
-        <v>17</v>
+        <v>110</v>
       </c>
       <c r="C147" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B148" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="C148" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A152" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B152" t="s">
+        <v>16</v>
+      </c>
+      <c r="C152" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B153" t="s">
+        <v>113</v>
+      </c>
+      <c r="C153" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B158" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B153" t="s">
-        <v>117</v>
-      </c>
-      <c r="C153" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B154" t="s">
-        <v>17</v>
-      </c>
-      <c r="C154" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B155" t="s">
-        <v>74</v>
-      </c>
-      <c r="C155" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B156" t="s">
+      <c r="C158" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B159" t="s">
+        <v>16</v>
+      </c>
+      <c r="C159" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B160" t="s">
+        <v>73</v>
+      </c>
+      <c r="C160" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B161" t="s">
         <v>3</v>
       </c>
-      <c r="C156" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B157" t="s">
-        <v>118</v>
-      </c>
-      <c r="C157" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B158" t="s">
-        <v>119</v>
-      </c>
-      <c r="C158" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B159" t="s">
-        <v>141</v>
-      </c>
-      <c r="C159" t="s">
-        <v>11</v>
-      </c>
-      <c r="E159" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A161" t="s">
-        <v>120</v>
+      <c r="C161" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B162" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C162" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B163" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C163" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B164" t="s">
-        <v>124</v>
+        <v>140</v>
       </c>
       <c r="C164" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B165" t="s">
-        <v>125</v>
-      </c>
-      <c r="C165" t="s">
-        <v>11</v>
-      </c>
-      <c r="E165" t="s">
-        <v>126</v>
+        <v>10</v>
+      </c>
+      <c r="E164" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B166" t="s">
-        <v>128</v>
-      </c>
-      <c r="C166" t="s">
-        <v>90</v>
-      </c>
-      <c r="E166" t="s">
-        <v>127</v>
+      <c r="A166" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B167" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="C167" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B168" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="C168" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B169" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="C169" t="s">
-        <v>11</v>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B170" t="s">
+        <v>124</v>
+      </c>
+      <c r="C170" t="s">
+        <v>10</v>
+      </c>
+      <c r="E170" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A171" t="s">
-        <v>121</v>
+      <c r="B171" t="s">
+        <v>127</v>
+      </c>
+      <c r="C171" t="s">
+        <v>89</v>
+      </c>
+      <c r="E171" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B172" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="C172" t="s">
         <v>10</v>
@@ -2039,7 +2101,7 @@
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B173" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="C173" t="s">
         <v>10</v>
@@ -2047,58 +2109,44 @@
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B174" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="C174" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B175" t="s">
-        <v>134</v>
-      </c>
-      <c r="C175" t="s">
-        <v>11</v>
-      </c>
-    </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B176" t="s">
-        <v>136</v>
-      </c>
-      <c r="C176" t="s">
-        <v>46</v>
+      <c r="A176" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B177" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C177" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B178" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="C178" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B179" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="C179" t="s">
-        <v>11</v>
-      </c>
-      <c r="E179" t="s">
-        <v>137</v>
+        <v>9</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B180" t="s">
-        <v>17</v>
+        <v>133</v>
       </c>
       <c r="C180" t="s">
         <v>10</v>
@@ -2106,92 +2154,188 @@
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B181" t="s">
-        <v>111</v>
+        <v>135</v>
       </c>
       <c r="C181" t="s">
-        <v>11</v>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B182" t="s">
+        <v>137</v>
+      </c>
+      <c r="C182" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B183" t="s">
+        <v>131</v>
+      </c>
+      <c r="C183" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A184" t="s">
-        <v>21</v>
+      <c r="B184" t="s">
+        <v>132</v>
+      </c>
+      <c r="C184" t="s">
+        <v>10</v>
+      </c>
+      <c r="E184" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B185" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="C185" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B186" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="C186" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B187" t="s">
-        <v>148</v>
-      </c>
-      <c r="C187" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B188" t="s">
-        <v>94</v>
+        <v>10</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B189" t="s">
-        <v>149</v>
+      <c r="A189" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B190" t="s">
-        <v>150</v>
+        <v>2</v>
+      </c>
+      <c r="C190" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B191" t="s">
-        <v>151</v>
+        <v>92</v>
+      </c>
+      <c r="C191" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B192" t="s">
-        <v>152</v>
+        <v>147</v>
+      </c>
+      <c r="C192" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B193" t="s">
-        <v>153</v>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B194" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B195" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A196" t="s">
-        <v>163</v>
+      <c r="B196" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B197" t="s">
-        <v>163</v>
-      </c>
-      <c r="C197" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B198" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>145</v>
+        <v>162</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B202" t="s">
+        <v>162</v>
+      </c>
+      <c r="C202" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B203" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A206" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B207" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B208" t="s">
+        <v>167</v>
+      </c>
+      <c r="C208" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="209" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B209" t="s">
+        <v>168</v>
+      </c>
+      <c r="C209" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="210" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B210" t="s">
+        <v>172</v>
+      </c>
+      <c r="C210" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="211" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B211" t="s">
+        <v>173</v>
+      </c>
+      <c r="C211" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="212" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B212" t="s">
+        <v>175</v>
+      </c>
+      <c r="C212" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="213" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B213" t="s">
+        <v>176</v>
+      </c>
+      <c r="C213" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>